<commit_message>
updated xlxs file, festival-api-routes, server.js
</commit_message>
<xml_diff>
--- a/documents/festival info.xlsx
+++ b/documents/festival info.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17927"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zamir\FestiVibez\BestFest\documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="1600" yWindow="0" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="77">
   <si>
     <t>Coachella</t>
   </si>
@@ -90,42 +95,15 @@
     <t>symbiosisgathering.com</t>
   </si>
   <si>
-    <t>reggaeontheriver.com</t>
-  </si>
-  <si>
-    <t>Kaaboodelmar.com</t>
-  </si>
-  <si>
-    <t>hardfest.com</t>
-  </si>
-  <si>
-    <t>snowglobemusicfestival.com/</t>
-  </si>
-  <si>
-    <t>beyondwonderland.com/</t>
-  </si>
-  <si>
     <t>https://www.desertheartsfestival.com/</t>
   </si>
   <si>
     <t>https://www.coachella.com/</t>
   </si>
   <si>
-    <t>lightninginabottle.org</t>
-  </si>
-  <si>
-    <t>sfoutsidelands.org</t>
-  </si>
-  <si>
     <t>crssdfest.com</t>
   </si>
   <si>
-    <t>stagecoachfest.com</t>
-  </si>
-  <si>
-    <t>fyffest.com</t>
-  </si>
-  <si>
     <t>Bradley, CA</t>
   </si>
   <si>
@@ -190,16 +168,114 @@
   </si>
   <si>
     <t>December 29-31</t>
+  </si>
+  <si>
+    <t>https://lightninginabottle.org</t>
+  </si>
+  <si>
+    <t>https://fyffest.com</t>
+  </si>
+  <si>
+    <t>https://Kaaboodelmar.com</t>
+  </si>
+  <si>
+    <t>https://hardfest.com</t>
+  </si>
+  <si>
+    <t>https://beyondwonderland.com/</t>
+  </si>
+  <si>
+    <t>http://snowglobemusicfestival.com/</t>
+  </si>
+  <si>
+    <t>http://www.reggaeontheriver.com/</t>
+  </si>
+  <si>
+    <t>http://www.stagecoachfestival.com/</t>
+  </si>
+  <si>
+    <t>https://www.sfoutsidelands.com/</t>
+  </si>
+  <si>
+    <t>Genre</t>
+  </si>
+  <si>
+    <t>Mixed</t>
+  </si>
+  <si>
+    <t>EDM/House</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Reggae</t>
+  </si>
+  <si>
+    <t>EDM</t>
+  </si>
+  <si>
+    <t>../assets/images/coachella.jpg</t>
+  </si>
+  <si>
+    <t>../assets/images/symbiosis.jpg</t>
+  </si>
+  <si>
+    <t>../assets/images/LIB.jpg</t>
+  </si>
+  <si>
+    <t>../assets/images/outsidelands.jpg</t>
+  </si>
+  <si>
+    <t>../assets/images/crssd.jpg</t>
+  </si>
+  <si>
+    <t>../assets/images/stagecoachjpg</t>
+  </si>
+  <si>
+    <t>../assets/images/fyffest.jpg</t>
+  </si>
+  <si>
+    <t>../assets/images/reggaeriver.jpg</t>
+  </si>
+  <si>
+    <t>../assets/images/kaboo.jpg</t>
+  </si>
+  <si>
+    <t>../assets/images/hardfest.jpg</t>
+  </si>
+  <si>
+    <t>../assets/images/snowglobe.jpg</t>
+  </si>
+  <si>
+    <t>../assets/images/beyondwonderland.jpg</t>
+  </si>
+  <si>
+    <t>../assets/images/deserthearts.jpg</t>
+  </si>
+  <si>
+    <t>Img url</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="\”@\”"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -222,17 +298,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -558,21 +646,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.08203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -588,230 +677,330 @@
       <c r="E1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="E14" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" t="s">
-        <v>28</v>
+      <c r="F14" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4" display="https://crssdfest.com"/>
+    <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="E7" r:id="rId6"/>
+    <hyperlink ref="E8" r:id="rId7" display="https://symbiosisgathering.com"/>
+    <hyperlink ref="E9" r:id="rId8"/>
+    <hyperlink ref="E10" r:id="rId9"/>
+    <hyperlink ref="E11" r:id="rId10"/>
+    <hyperlink ref="E12" r:id="rId11"/>
+    <hyperlink ref="E13" r:id="rId12"/>
+    <hyperlink ref="E14" r:id="rId13"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
summary added to xl file
</commit_message>
<xml_diff>
--- a/documents/festival info.xlsx
+++ b/documents/festival info.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zamir\FestiVibez\BestFest\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zamir\festi project\BestFest\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="80">
   <si>
     <t>Coachella</t>
   </si>
@@ -255,6 +255,15 @@
   </si>
   <si>
     <t>Img url</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Curabitur pharetra interdum egestas. Vestibulum luctus lacus eget quam laoreet posuere. Nam volutpat, mi at facilisis egestas, diam elit aliquam neque, vitae tempus diam nulla nec elit. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lorem ipsum dolor sit amet, consectetur adipiscing elit. Curabitur pharetra interdum egestas. Vestibulum luctus lacus eget quam laoreet posuere. Nam volutpat, mi at facilisis egestas, diam elit aliquam neque, vitae tempus diam nulla nec elit. </t>
   </si>
 </sst>
 </file>
@@ -264,7 +273,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\”@\”"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -278,6 +287,14 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -302,10 +319,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -646,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -659,9 +679,10 @@
     <col min="3" max="3" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="36.08203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -683,8 +704,11 @@
       <c r="G1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -706,8 +730,11 @@
       <c r="G2" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -729,8 +756,11 @@
       <c r="G3" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -752,8 +782,11 @@
       <c r="G4" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -775,8 +808,11 @@
       <c r="G5" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H5" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -798,8 +834,11 @@
       <c r="G6" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -821,8 +860,11 @@
       <c r="G7" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H7" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -844,8 +886,11 @@
       <c r="G8" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -867,8 +912,11 @@
       <c r="G9" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H9" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -890,8 +938,11 @@
       <c r="G10" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H10" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -913,8 +964,11 @@
       <c r="G11" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H11" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -936,8 +990,11 @@
       <c r="G12" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H12" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -959,8 +1016,11 @@
       <c r="G13" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H13" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -981,6 +1041,9 @@
       </c>
       <c r="G14" s="2" t="s">
         <v>75</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
touppercase and xlxs fix for image links
</commit_message>
<xml_diff>
--- a/documents/festival info.xlsx
+++ b/documents/festival info.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -230,18 +230,12 @@
     <t>../assets/images/crssd.jpg</t>
   </si>
   <si>
-    <t>../assets/images/stagecoachjpg</t>
-  </si>
-  <si>
     <t>../assets/images/fyffest.jpg</t>
   </si>
   <si>
     <t>../assets/images/reggaeriver.jpg</t>
   </si>
   <si>
-    <t>../assets/images/kaboo.jpg</t>
-  </si>
-  <si>
     <t>../assets/images/hardfest.jpg</t>
   </si>
   <si>
@@ -264,6 +258,12 @@
   </si>
   <si>
     <t xml:space="preserve">Lorem ipsum dolor sit amet, consectetur adipiscing elit. Curabitur pharetra interdum egestas. Vestibulum luctus lacus eget quam laoreet posuere. Nam volutpat, mi at facilisis egestas, diam elit aliquam neque, vitae tempus diam nulla nec elit. </t>
+  </si>
+  <si>
+    <t>../assets/images/kaaboodelmar.jpg</t>
+  </si>
+  <si>
+    <t>../assets/images/stagecoach.jpg</t>
   </si>
 </sst>
 </file>
@@ -668,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -702,10 +702,10 @@
         <v>57</v>
       </c>
       <c r="G1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
@@ -731,7 +731,7 @@
         <v>63</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
@@ -757,7 +757,7 @@
         <v>65</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
@@ -783,7 +783,7 @@
         <v>66</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
@@ -809,7 +809,7 @@
         <v>67</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
@@ -832,10 +832,10 @@
         <v>60</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
@@ -858,10 +858,10 @@
         <v>58</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
@@ -887,7 +887,7 @@
         <v>64</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
@@ -910,10 +910,10 @@
         <v>61</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
@@ -936,10 +936,10 @@
         <v>58</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
@@ -962,10 +962,10 @@
         <v>62</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
@@ -988,10 +988,10 @@
         <v>58</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
@@ -1014,10 +1014,10 @@
         <v>62</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -1040,10 +1040,10 @@
         <v>62</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>